<commit_message>
Changed the plots for the number of pixels
</commit_message>
<xml_diff>
--- a/Testing/results/NoOfPixels_DataUniqueClasses.xlsx
+++ b/Testing/results/NoOfPixels_DataUniqueClasses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anant\Desktop\ATLAS_ontology\github\ORATOR-ATLAS\Testing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39CBBBF-0B36-4B45-87DF-100C7AEC85C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EBECB9-E557-4651-A7F9-16E9CEF8B42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5190" windowWidth="29040" windowHeight="15720" tabRatio="795" xr2:uid="{CE8EB44D-63BF-455D-AE7E-30E9BC4D19F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="795" firstSheet="5" activeTab="5" xr2:uid="{CE8EB44D-63BF-455D-AE7E-30E9BC4D19F1}"/>
   </bookViews>
   <sheets>
     <sheet name="pixelPerClassInDataset_RELLIS" sheetId="2" r:id="rId1"/>
@@ -271,9 +271,6 @@
     <t>rubble</t>
   </si>
   <si>
-    <t>unknown_error</t>
-  </si>
-  <si>
     <t>trail</t>
   </si>
   <si>
@@ -283,18 +280,12 @@
     <t>sand</t>
   </si>
   <si>
-    <t>container_and_generic_object</t>
-  </si>
-  <si>
     <t>gravel</t>
   </si>
   <si>
     <t>mulch</t>
   </si>
   <si>
-    <t>rock_bed</t>
-  </si>
-  <si>
     <t>bicyle</t>
   </si>
   <si>
@@ -307,27 +298,12 @@
     <t>bridge</t>
   </si>
   <si>
-    <t>picnic_table</t>
-  </si>
-  <si>
     <t>background</t>
   </si>
   <si>
-    <t>smooth_trail</t>
-  </si>
-  <si>
-    <t>rough_trail</t>
-  </si>
-  <si>
     <t>obstacle</t>
   </si>
   <si>
-    <t>low_vegetation</t>
-  </si>
-  <si>
-    <t>high_vegetation</t>
-  </si>
-  <si>
     <t>'Nature_object'</t>
   </si>
   <si>
@@ -499,109 +475,133 @@
     <t>truck</t>
   </si>
   <si>
-    <t>traffic_signs</t>
-  </si>
-  <si>
-    <t>Nature_object</t>
-  </si>
-  <si>
-    <t>RD_normal_street</t>
-  </si>
-  <si>
     <t>Sidewalk</t>
   </si>
   <si>
-    <t>Grid_structure</t>
-  </si>
-  <si>
-    <t>Road_blocks</t>
-  </si>
-  <si>
-    <t>Drivable_cobblestone</t>
-  </si>
-  <si>
     <t>Curbstone</t>
   </si>
   <si>
-    <t>Solid_line</t>
-  </si>
-  <si>
-    <t>Non_drivable_street</t>
-  </si>
-  <si>
     <t>Poles</t>
   </si>
   <si>
-    <t>Dashed_line</t>
-  </si>
-  <si>
-    <t>Irrelevant_signs</t>
-  </si>
-  <si>
-    <t>Parking_area</t>
-  </si>
-  <si>
-    <t>Obstacles_trash</t>
-  </si>
-  <si>
-    <t>RD_restricted_area</t>
-  </si>
-  <si>
-    <t>Traffic_guide_obj</t>
-  </si>
-  <si>
-    <t>Slow_drive_area</t>
-  </si>
-  <si>
-    <t>Signal_corpus</t>
-  </si>
-  <si>
-    <t>Painted_driv_instr</t>
-  </si>
-  <si>
     <t>Sidebars</t>
   </si>
   <si>
-    <t>Zebra_crossing</t>
-  </si>
-  <si>
-    <t>Electronic_traffic</t>
-  </si>
-  <si>
     <t>Tractor</t>
   </si>
   <si>
-    <t>Blurred_area</t>
-  </si>
-  <si>
     <t>Animals</t>
   </si>
   <si>
-    <t>Speed_bumper</t>
-  </si>
-  <si>
-    <t>Rain_dirt</t>
-  </si>
-  <si>
-    <t>Ego_car</t>
-  </si>
-  <si>
     <t>Pedestrian</t>
   </si>
   <si>
     <t>Bicycle</t>
   </si>
   <si>
-    <t>Utility_vehicle</t>
-  </si>
-  <si>
-    <t>Traffic_signal</t>
-  </si>
-  <si>
-    <t>Small_vehicles</t>
-  </si>
-  <si>
     <t>FREIBURG</t>
+  </si>
+  <si>
+    <t>Nature object</t>
+  </si>
+  <si>
+    <t>RD normal street</t>
+  </si>
+  <si>
+    <t>Ego car</t>
+  </si>
+  <si>
+    <t>Grid structure</t>
+  </si>
+  <si>
+    <t>Road blocks</t>
+  </si>
+  <si>
+    <t>Drivable cobblestone</t>
+  </si>
+  <si>
+    <t>Solid line</t>
+  </si>
+  <si>
+    <t>Non drivable street</t>
+  </si>
+  <si>
+    <t>Dashed line</t>
+  </si>
+  <si>
+    <t>Irrelevant signs</t>
+  </si>
+  <si>
+    <t>traffic signs</t>
+  </si>
+  <si>
+    <t>Parking area</t>
+  </si>
+  <si>
+    <t>Obstacles trash</t>
+  </si>
+  <si>
+    <t>high vegetation</t>
+  </si>
+  <si>
+    <t>RD restricted area</t>
+  </si>
+  <si>
+    <t>Traffic guide obj</t>
+  </si>
+  <si>
+    <t>Painted driv instr</t>
+  </si>
+  <si>
+    <t>Slow drive area</t>
+  </si>
+  <si>
+    <t>Signal corpus</t>
+  </si>
+  <si>
+    <t>rough trail</t>
+  </si>
+  <si>
+    <t>smooth trail</t>
+  </si>
+  <si>
+    <t>Utility vehicle</t>
+  </si>
+  <si>
+    <t>rock bed</t>
+  </si>
+  <si>
+    <t>Traffic signal</t>
+  </si>
+  <si>
+    <t>low vegetation</t>
+  </si>
+  <si>
+    <t>unknown error</t>
+  </si>
+  <si>
+    <t>Zebra crossing</t>
+  </si>
+  <si>
+    <t>Small vehicles</t>
+  </si>
+  <si>
+    <t>Electronic traffic</t>
+  </si>
+  <si>
+    <t>container &amp; generic object</t>
+  </si>
+  <si>
+    <t>picnic table</t>
+  </si>
+  <si>
+    <t>Blurred area</t>
+  </si>
+  <si>
+    <t>Speed bumper</t>
+  </si>
+  <si>
+    <t>Rain dirt</t>
   </si>
 </sst>
 </file>
@@ -716,32 +716,41 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="+mj-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:rPr lang="en-US" sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="50000"/>
                     <a:lumOff val="50000"/>
                   </a:sysClr>
                 </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
               </a:rPr>
-              <a:t>Number of Pixels in each unique class defined for each dataset </a:t>
+              <a:t>Number of Pixels in Each Unique Class as Defined by Each Dataset </a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2403669517607884"/>
+          <c:y val="5.4479692768941206E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -769,14 +778,14 @@
             <a:buFontTx/>
             <a:buNone/>
             <a:tabLst/>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:sysClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="+mj-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -830,236 +839,236 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>AllDatasets!$A$2:$A$77</c:f>
+              <c:f>AllDatasets!$H$2:$H$77</c:f>
               <c:strCache>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>sky</c:v>
+                  <c:v>Sky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nature_object</c:v>
+                  <c:v>Nature Object</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RD_normal_street</c:v>
+                  <c:v>Rd Normal Street</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>building</c:v>
+                  <c:v>Building</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>grass</c:v>
+                  <c:v>Grass</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>car</c:v>
+                  <c:v>Car</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>tree</c:v>
+                  <c:v>Tree</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>bush</c:v>
+                  <c:v>Bush</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sidewalk</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Ego_car</c:v>
+                  <c:v>Ego Car</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>truck</c:v>
+                  <c:v>Truck</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Grid_structure</c:v>
+                  <c:v>Grid Structure</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Road_blocks</c:v>
+                  <c:v>Road Blocks</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Drivable_cobblestone</c:v>
+                  <c:v>Drivable Cobblestone</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>Curbstone</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Solid_line</c:v>
+                  <c:v>Solid Line</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Non_drivable_street</c:v>
+                  <c:v>Non Drivable Street</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Dashed_line</c:v>
+                  <c:v>Dashed Line</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Poles</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Irrelevant_signs</c:v>
+                  <c:v>Irrelevant Signs</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>mud</c:v>
+                  <c:v>Mud</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>traffic_signs</c:v>
+                  <c:v>Traffic Signs</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>mulch</c:v>
+                  <c:v>Mulch</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Parking_area</c:v>
+                  <c:v>Parking Area</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>concrete</c:v>
+                  <c:v>Concrete</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Obstacles_trash</c:v>
+                  <c:v>Obstacles Trash</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>high_vegetation</c:v>
+                  <c:v>High Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>RD_restricted_area</c:v>
+                  <c:v>Rd Restricted Area</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>gravel</c:v>
+                  <c:v>Gravel</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Traffic_guide_obj</c:v>
+                  <c:v>Traffic Guide Obj</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>void</c:v>
+                  <c:v>Void</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Painted_driv_instr</c:v>
+                  <c:v>Painted Driv Instr</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Slow_drive_area</c:v>
+                  <c:v>Slow Drive Area</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>puddle</c:v>
+                  <c:v>Puddle</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Signal_corpus</c:v>
+                  <c:v>Signal Corpus</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>Pedestrian</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>rough_trail</c:v>
+                  <c:v>Rough Trail</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>smooth_trail</c:v>
+                  <c:v>Smooth Trail</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>Bicycle</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>Utility_vehicle</c:v>
+                  <c:v>Utility Vehicle</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>vegetation</c:v>
+                  <c:v>Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>rock_bed</c:v>
+                  <c:v>Rock Bed</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>barrier</c:v>
+                  <c:v>Barrier</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>Traffic_signal</c:v>
+                  <c:v>Traffic Signal</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>asphalt</c:v>
+                  <c:v>Asphalt</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>Sidebars</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>low_vegetation</c:v>
+                  <c:v>Low Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>rubble</c:v>
+                  <c:v>Rubble</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>fence</c:v>
+                  <c:v>Fence</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>vehicle</c:v>
+                  <c:v>Vehicle</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>water</c:v>
+                  <c:v>Water</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>unknown_error</c:v>
+                  <c:v>Unknown Error</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>Zebra_crossing</c:v>
+                  <c:v>Zebra Crossing</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>background</c:v>
+                  <c:v>Background</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>log</c:v>
+                  <c:v>Log</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>trail</c:v>
+                  <c:v>Trail</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>person</c:v>
+                  <c:v>Person</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>Small_vehicles</c:v>
+                  <c:v>Small Vehicles</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>obstacle</c:v>
+                  <c:v>Obstacle</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>dirt</c:v>
+                  <c:v>Dirt</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>bridge</c:v>
+                  <c:v>Bridge</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>object</c:v>
+                  <c:v>Object</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>pole</c:v>
+                  <c:v>Pole</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>log</c:v>
+                  <c:v>Log</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>Electronic_traffic</c:v>
+                  <c:v>Electronic Traffic</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>sand</c:v>
+                  <c:v>Sand</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>rock</c:v>
+                  <c:v>Rock</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>container_and_generic_object</c:v>
+                  <c:v>Container &amp; Generic Object</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>picnic_table</c:v>
+                  <c:v>Picnic Table</c:v>
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>Tractor</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>Blurred_area</c:v>
+                  <c:v>Blurred Area</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>Animals</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>sign</c:v>
+                  <c:v>Sign</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>bicyle</c:v>
+                  <c:v>Bicyle</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>Speed_bumper</c:v>
+                  <c:v>Speed Bumper</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>Rain_dirt</c:v>
+                  <c:v>Rain Dirt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1170,236 +1179,236 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>AllDatasets!$A$2:$A$77</c:f>
+              <c:f>AllDatasets!$H$2:$H$77</c:f>
               <c:strCache>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>sky</c:v>
+                  <c:v>Sky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nature_object</c:v>
+                  <c:v>Nature Object</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RD_normal_street</c:v>
+                  <c:v>Rd Normal Street</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>building</c:v>
+                  <c:v>Building</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>grass</c:v>
+                  <c:v>Grass</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>car</c:v>
+                  <c:v>Car</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>tree</c:v>
+                  <c:v>Tree</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>bush</c:v>
+                  <c:v>Bush</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sidewalk</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Ego_car</c:v>
+                  <c:v>Ego Car</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>truck</c:v>
+                  <c:v>Truck</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Grid_structure</c:v>
+                  <c:v>Grid Structure</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Road_blocks</c:v>
+                  <c:v>Road Blocks</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Drivable_cobblestone</c:v>
+                  <c:v>Drivable Cobblestone</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>Curbstone</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Solid_line</c:v>
+                  <c:v>Solid Line</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Non_drivable_street</c:v>
+                  <c:v>Non Drivable Street</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Dashed_line</c:v>
+                  <c:v>Dashed Line</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Poles</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Irrelevant_signs</c:v>
+                  <c:v>Irrelevant Signs</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>mud</c:v>
+                  <c:v>Mud</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>traffic_signs</c:v>
+                  <c:v>Traffic Signs</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>mulch</c:v>
+                  <c:v>Mulch</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Parking_area</c:v>
+                  <c:v>Parking Area</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>concrete</c:v>
+                  <c:v>Concrete</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Obstacles_trash</c:v>
+                  <c:v>Obstacles Trash</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>high_vegetation</c:v>
+                  <c:v>High Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>RD_restricted_area</c:v>
+                  <c:v>Rd Restricted Area</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>gravel</c:v>
+                  <c:v>Gravel</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Traffic_guide_obj</c:v>
+                  <c:v>Traffic Guide Obj</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>void</c:v>
+                  <c:v>Void</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Painted_driv_instr</c:v>
+                  <c:v>Painted Driv Instr</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Slow_drive_area</c:v>
+                  <c:v>Slow Drive Area</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>puddle</c:v>
+                  <c:v>Puddle</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Signal_corpus</c:v>
+                  <c:v>Signal Corpus</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>Pedestrian</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>rough_trail</c:v>
+                  <c:v>Rough Trail</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>smooth_trail</c:v>
+                  <c:v>Smooth Trail</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>Bicycle</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>Utility_vehicle</c:v>
+                  <c:v>Utility Vehicle</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>vegetation</c:v>
+                  <c:v>Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>rock_bed</c:v>
+                  <c:v>Rock Bed</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>barrier</c:v>
+                  <c:v>Barrier</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>Traffic_signal</c:v>
+                  <c:v>Traffic Signal</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>asphalt</c:v>
+                  <c:v>Asphalt</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>Sidebars</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>low_vegetation</c:v>
+                  <c:v>Low Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>rubble</c:v>
+                  <c:v>Rubble</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>fence</c:v>
+                  <c:v>Fence</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>vehicle</c:v>
+                  <c:v>Vehicle</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>water</c:v>
+                  <c:v>Water</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>unknown_error</c:v>
+                  <c:v>Unknown Error</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>Zebra_crossing</c:v>
+                  <c:v>Zebra Crossing</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>background</c:v>
+                  <c:v>Background</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>log</c:v>
+                  <c:v>Log</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>trail</c:v>
+                  <c:v>Trail</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>person</c:v>
+                  <c:v>Person</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>Small_vehicles</c:v>
+                  <c:v>Small Vehicles</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>obstacle</c:v>
+                  <c:v>Obstacle</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>dirt</c:v>
+                  <c:v>Dirt</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>bridge</c:v>
+                  <c:v>Bridge</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>object</c:v>
+                  <c:v>Object</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>pole</c:v>
+                  <c:v>Pole</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>log</c:v>
+                  <c:v>Log</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>Electronic_traffic</c:v>
+                  <c:v>Electronic Traffic</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>sand</c:v>
+                  <c:v>Sand</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>rock</c:v>
+                  <c:v>Rock</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>container_and_generic_object</c:v>
+                  <c:v>Container &amp; Generic Object</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>picnic_table</c:v>
+                  <c:v>Picnic Table</c:v>
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>Tractor</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>Blurred_area</c:v>
+                  <c:v>Blurred Area</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>Animals</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>sign</c:v>
+                  <c:v>Sign</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>bicyle</c:v>
+                  <c:v>Bicyle</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>Speed_bumper</c:v>
+                  <c:v>Speed Bumper</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>Rain_dirt</c:v>
+                  <c:v>Rain Dirt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1477,236 +1486,236 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>AllDatasets!$A$2:$A$77</c:f>
+              <c:f>AllDatasets!$H$2:$H$77</c:f>
               <c:strCache>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>sky</c:v>
+                  <c:v>Sky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nature_object</c:v>
+                  <c:v>Nature Object</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RD_normal_street</c:v>
+                  <c:v>Rd Normal Street</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>building</c:v>
+                  <c:v>Building</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>grass</c:v>
+                  <c:v>Grass</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>car</c:v>
+                  <c:v>Car</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>tree</c:v>
+                  <c:v>Tree</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>bush</c:v>
+                  <c:v>Bush</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sidewalk</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Ego_car</c:v>
+                  <c:v>Ego Car</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>truck</c:v>
+                  <c:v>Truck</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Grid_structure</c:v>
+                  <c:v>Grid Structure</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Road_blocks</c:v>
+                  <c:v>Road Blocks</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Drivable_cobblestone</c:v>
+                  <c:v>Drivable Cobblestone</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>Curbstone</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Solid_line</c:v>
+                  <c:v>Solid Line</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Non_drivable_street</c:v>
+                  <c:v>Non Drivable Street</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Dashed_line</c:v>
+                  <c:v>Dashed Line</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Poles</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Irrelevant_signs</c:v>
+                  <c:v>Irrelevant Signs</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>mud</c:v>
+                  <c:v>Mud</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>traffic_signs</c:v>
+                  <c:v>Traffic Signs</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>mulch</c:v>
+                  <c:v>Mulch</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Parking_area</c:v>
+                  <c:v>Parking Area</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>concrete</c:v>
+                  <c:v>Concrete</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Obstacles_trash</c:v>
+                  <c:v>Obstacles Trash</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>high_vegetation</c:v>
+                  <c:v>High Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>RD_restricted_area</c:v>
+                  <c:v>Rd Restricted Area</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>gravel</c:v>
+                  <c:v>Gravel</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Traffic_guide_obj</c:v>
+                  <c:v>Traffic Guide Obj</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>void</c:v>
+                  <c:v>Void</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Painted_driv_instr</c:v>
+                  <c:v>Painted Driv Instr</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Slow_drive_area</c:v>
+                  <c:v>Slow Drive Area</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>puddle</c:v>
+                  <c:v>Puddle</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Signal_corpus</c:v>
+                  <c:v>Signal Corpus</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>Pedestrian</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>rough_trail</c:v>
+                  <c:v>Rough Trail</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>smooth_trail</c:v>
+                  <c:v>Smooth Trail</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>Bicycle</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>Utility_vehicle</c:v>
+                  <c:v>Utility Vehicle</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>vegetation</c:v>
+                  <c:v>Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>rock_bed</c:v>
+                  <c:v>Rock Bed</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>barrier</c:v>
+                  <c:v>Barrier</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>Traffic_signal</c:v>
+                  <c:v>Traffic Signal</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>asphalt</c:v>
+                  <c:v>Asphalt</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>Sidebars</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>low_vegetation</c:v>
+                  <c:v>Low Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>rubble</c:v>
+                  <c:v>Rubble</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>fence</c:v>
+                  <c:v>Fence</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>vehicle</c:v>
+                  <c:v>Vehicle</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>water</c:v>
+                  <c:v>Water</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>unknown_error</c:v>
+                  <c:v>Unknown Error</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>Zebra_crossing</c:v>
+                  <c:v>Zebra Crossing</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>background</c:v>
+                  <c:v>Background</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>log</c:v>
+                  <c:v>Log</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>trail</c:v>
+                  <c:v>Trail</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>person</c:v>
+                  <c:v>Person</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>Small_vehicles</c:v>
+                  <c:v>Small Vehicles</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>obstacle</c:v>
+                  <c:v>Obstacle</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>dirt</c:v>
+                  <c:v>Dirt</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>bridge</c:v>
+                  <c:v>Bridge</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>object</c:v>
+                  <c:v>Object</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>pole</c:v>
+                  <c:v>Pole</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>log</c:v>
+                  <c:v>Log</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>Electronic_traffic</c:v>
+                  <c:v>Electronic Traffic</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>sand</c:v>
+                  <c:v>Sand</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>rock</c:v>
+                  <c:v>Rock</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>container_and_generic_object</c:v>
+                  <c:v>Container &amp; Generic Object</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>picnic_table</c:v>
+                  <c:v>Picnic Table</c:v>
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>Tractor</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>Blurred_area</c:v>
+                  <c:v>Blurred Area</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>Animals</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>sign</c:v>
+                  <c:v>Sign</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>bicyle</c:v>
+                  <c:v>Bicyle</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>Speed_bumper</c:v>
+                  <c:v>Speed Bumper</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>Rain_dirt</c:v>
+                  <c:v>Rain Dirt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1772,236 +1781,236 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>AllDatasets!$A$2:$A$77</c:f>
+              <c:f>AllDatasets!$H$2:$H$77</c:f>
               <c:strCache>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>sky</c:v>
+                  <c:v>Sky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nature_object</c:v>
+                  <c:v>Nature Object</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RD_normal_street</c:v>
+                  <c:v>Rd Normal Street</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>building</c:v>
+                  <c:v>Building</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>grass</c:v>
+                  <c:v>Grass</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>car</c:v>
+                  <c:v>Car</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>tree</c:v>
+                  <c:v>Tree</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>bush</c:v>
+                  <c:v>Bush</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sidewalk</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Ego_car</c:v>
+                  <c:v>Ego Car</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>truck</c:v>
+                  <c:v>Truck</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Grid_structure</c:v>
+                  <c:v>Grid Structure</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Road_blocks</c:v>
+                  <c:v>Road Blocks</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Drivable_cobblestone</c:v>
+                  <c:v>Drivable Cobblestone</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>Curbstone</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Solid_line</c:v>
+                  <c:v>Solid Line</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Non_drivable_street</c:v>
+                  <c:v>Non Drivable Street</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Dashed_line</c:v>
+                  <c:v>Dashed Line</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Poles</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Irrelevant_signs</c:v>
+                  <c:v>Irrelevant Signs</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>mud</c:v>
+                  <c:v>Mud</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>traffic_signs</c:v>
+                  <c:v>Traffic Signs</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>mulch</c:v>
+                  <c:v>Mulch</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Parking_area</c:v>
+                  <c:v>Parking Area</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>concrete</c:v>
+                  <c:v>Concrete</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Obstacles_trash</c:v>
+                  <c:v>Obstacles Trash</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>high_vegetation</c:v>
+                  <c:v>High Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>RD_restricted_area</c:v>
+                  <c:v>Rd Restricted Area</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>gravel</c:v>
+                  <c:v>Gravel</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Traffic_guide_obj</c:v>
+                  <c:v>Traffic Guide Obj</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>void</c:v>
+                  <c:v>Void</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Painted_driv_instr</c:v>
+                  <c:v>Painted Driv Instr</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Slow_drive_area</c:v>
+                  <c:v>Slow Drive Area</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>puddle</c:v>
+                  <c:v>Puddle</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Signal_corpus</c:v>
+                  <c:v>Signal Corpus</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>Pedestrian</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>rough_trail</c:v>
+                  <c:v>Rough Trail</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>smooth_trail</c:v>
+                  <c:v>Smooth Trail</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>Bicycle</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>Utility_vehicle</c:v>
+                  <c:v>Utility Vehicle</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>vegetation</c:v>
+                  <c:v>Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>rock_bed</c:v>
+                  <c:v>Rock Bed</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>barrier</c:v>
+                  <c:v>Barrier</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>Traffic_signal</c:v>
+                  <c:v>Traffic Signal</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>asphalt</c:v>
+                  <c:v>Asphalt</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>Sidebars</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>low_vegetation</c:v>
+                  <c:v>Low Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>rubble</c:v>
+                  <c:v>Rubble</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>fence</c:v>
+                  <c:v>Fence</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>vehicle</c:v>
+                  <c:v>Vehicle</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>water</c:v>
+                  <c:v>Water</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>unknown_error</c:v>
+                  <c:v>Unknown Error</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>Zebra_crossing</c:v>
+                  <c:v>Zebra Crossing</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>background</c:v>
+                  <c:v>Background</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>log</c:v>
+                  <c:v>Log</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>trail</c:v>
+                  <c:v>Trail</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>person</c:v>
+                  <c:v>Person</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>Small_vehicles</c:v>
+                  <c:v>Small Vehicles</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>obstacle</c:v>
+                  <c:v>Obstacle</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>dirt</c:v>
+                  <c:v>Dirt</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>bridge</c:v>
+                  <c:v>Bridge</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>object</c:v>
+                  <c:v>Object</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>pole</c:v>
+                  <c:v>Pole</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>log</c:v>
+                  <c:v>Log</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>Electronic_traffic</c:v>
+                  <c:v>Electronic Traffic</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>sand</c:v>
+                  <c:v>Sand</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>rock</c:v>
+                  <c:v>Rock</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>container_and_generic_object</c:v>
+                  <c:v>Container &amp; Generic Object</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>picnic_table</c:v>
+                  <c:v>Picnic Table</c:v>
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>Tractor</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>Blurred_area</c:v>
+                  <c:v>Blurred Area</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>Animals</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>sign</c:v>
+                  <c:v>Sign</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>bicyle</c:v>
+                  <c:v>Bicyle</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>Speed_bumper</c:v>
+                  <c:v>Speed Bumper</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>Rain_dirt</c:v>
+                  <c:v>Rain Dirt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2127,236 +2136,236 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>AllDatasets!$A$2:$A$77</c:f>
+              <c:f>AllDatasets!$H$2:$H$77</c:f>
               <c:strCache>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>sky</c:v>
+                  <c:v>Sky</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nature_object</c:v>
+                  <c:v>Nature Object</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>RD_normal_street</c:v>
+                  <c:v>Rd Normal Street</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>building</c:v>
+                  <c:v>Building</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>grass</c:v>
+                  <c:v>Grass</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>car</c:v>
+                  <c:v>Car</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>tree</c:v>
+                  <c:v>Tree</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>bush</c:v>
+                  <c:v>Bush</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Sidewalk</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Ego_car</c:v>
+                  <c:v>Ego Car</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>truck</c:v>
+                  <c:v>Truck</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Grid_structure</c:v>
+                  <c:v>Grid Structure</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Road_blocks</c:v>
+                  <c:v>Road Blocks</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Drivable_cobblestone</c:v>
+                  <c:v>Drivable Cobblestone</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>Curbstone</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Solid_line</c:v>
+                  <c:v>Solid Line</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Non_drivable_street</c:v>
+                  <c:v>Non Drivable Street</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Dashed_line</c:v>
+                  <c:v>Dashed Line</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Poles</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Irrelevant_signs</c:v>
+                  <c:v>Irrelevant Signs</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>mud</c:v>
+                  <c:v>Mud</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>traffic_signs</c:v>
+                  <c:v>Traffic Signs</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>mulch</c:v>
+                  <c:v>Mulch</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>Parking_area</c:v>
+                  <c:v>Parking Area</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>concrete</c:v>
+                  <c:v>Concrete</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Obstacles_trash</c:v>
+                  <c:v>Obstacles Trash</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>high_vegetation</c:v>
+                  <c:v>High Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>RD_restricted_area</c:v>
+                  <c:v>Rd Restricted Area</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>gravel</c:v>
+                  <c:v>Gravel</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Traffic_guide_obj</c:v>
+                  <c:v>Traffic Guide Obj</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>void</c:v>
+                  <c:v>Void</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>Painted_driv_instr</c:v>
+                  <c:v>Painted Driv Instr</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>Slow_drive_area</c:v>
+                  <c:v>Slow Drive Area</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>puddle</c:v>
+                  <c:v>Puddle</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>Signal_corpus</c:v>
+                  <c:v>Signal Corpus</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>Pedestrian</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>rough_trail</c:v>
+                  <c:v>Rough Trail</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>smooth_trail</c:v>
+                  <c:v>Smooth Trail</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>Bicycle</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>Utility_vehicle</c:v>
+                  <c:v>Utility Vehicle</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>vegetation</c:v>
+                  <c:v>Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>rock_bed</c:v>
+                  <c:v>Rock Bed</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>barrier</c:v>
+                  <c:v>Barrier</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>Traffic_signal</c:v>
+                  <c:v>Traffic Signal</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>asphalt</c:v>
+                  <c:v>Asphalt</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>Sidebars</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>low_vegetation</c:v>
+                  <c:v>Low Vegetation</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>rubble</c:v>
+                  <c:v>Rubble</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>fence</c:v>
+                  <c:v>Fence</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>vehicle</c:v>
+                  <c:v>Vehicle</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>water</c:v>
+                  <c:v>Water</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>unknown_error</c:v>
+                  <c:v>Unknown Error</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>Zebra_crossing</c:v>
+                  <c:v>Zebra Crossing</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>background</c:v>
+                  <c:v>Background</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>log</c:v>
+                  <c:v>Log</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>trail</c:v>
+                  <c:v>Trail</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>person</c:v>
+                  <c:v>Person</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>Small_vehicles</c:v>
+                  <c:v>Small Vehicles</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>obstacle</c:v>
+                  <c:v>Obstacle</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>dirt</c:v>
+                  <c:v>Dirt</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>bridge</c:v>
+                  <c:v>Bridge</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>object</c:v>
+                  <c:v>Object</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>pole</c:v>
+                  <c:v>Pole</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>log</c:v>
+                  <c:v>Log</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>Electronic_traffic</c:v>
+                  <c:v>Electronic Traffic</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>sand</c:v>
+                  <c:v>Sand</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>rock</c:v>
+                  <c:v>Rock</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>container_and_generic_object</c:v>
+                  <c:v>Container &amp; Generic Object</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>picnic_table</c:v>
+                  <c:v>Picnic Table</c:v>
                 </c:pt>
                 <c:pt idx="69">
                   <c:v>Tractor</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>Blurred_area</c:v>
+                  <c:v>Blurred Area</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>Animals</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>sign</c:v>
+                  <c:v>Sign</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>bicyle</c:v>
+                  <c:v>Bicyle</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>Speed_bumper</c:v>
+                  <c:v>Speed Bumper</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>Rain_dirt</c:v>
+                  <c:v>Rain Dirt</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2531,7 +2540,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2597,7 +2606,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2632,9 +2641,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.73551020798790301"/>
-          <c:y val="9.4340411502564905E-2"/>
-          <c:w val="0.23318046486356411"/>
+          <c:x val="0.66849202501013372"/>
+          <c:y val="0.12523375284684363"/>
+          <c:w val="0.31500495119553362"/>
           <c:h val="0.11429774577049179"/>
         </c:manualLayout>
       </c:layout>
@@ -2651,7 +2660,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3258,16 +3267,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>105459</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>42415</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>991283</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>80514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>229083</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>117665</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3704,17 +3713,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE29B7C-20E5-42D6-AF34-FA28CA7AB762}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3722,7 +3731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3730,7 +3739,7 @@
         <v>133543140</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3738,7 +3747,7 @@
         <v>10059</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3746,7 +3755,7 @@
         <v>4784116443</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3754,7 +3763,7 @@
         <v>1997329017</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3762,7 +3771,7 @@
         <v>2501915</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3770,7 +3779,7 @@
         <v>11811153</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3778,7 +3787,7 @@
         <v>4210629590</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3786,7 +3795,7 @@
         <v>4889322</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -3794,7 +3803,7 @@
         <v>4412551</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -3802,7 +3811,7 @@
         <v>8324994</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3810,7 +3819,7 @@
         <v>3438186</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3818,7 +3827,7 @@
         <v>4718316</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3826,7 +3835,7 @@
         <v>8791996</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -3834,7 +3843,7 @@
         <v>4445609</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -3842,7 +3851,7 @@
         <v>2460720650</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -3850,7 +3859,7 @@
         <v>221680148</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -3858,7 +3867,7 @@
         <v>53338450</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -3866,7 +3875,7 @@
         <v>111981143</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -3874,7 +3883,7 @@
         <v>350542071</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -3882,7 +3891,7 @@
         <v>26891615</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3906,13 +3915,13 @@
       <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3920,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3928,7 +3937,7 @@
         <v>441762</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -3936,7 +3945,7 @@
         <v>13732978</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3944,7 +3953,7 @@
         <v>39719160</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3952,7 +3961,7 @@
         <v>34739739</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -3960,7 +3969,7 @@
         <v>61190727</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -3984,13 +3993,13 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3998,7 +4007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4006,7 +4015,7 @@
         <v>397879</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4014,7 +4023,7 @@
         <v>5133510</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -4022,7 +4031,7 @@
         <v>4512457</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4030,7 +4039,7 @@
         <v>632645350</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4038,7 +4047,7 @@
         <v>1102869439</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4046,7 +4055,7 @@
         <v>2299774</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4054,7 +4063,7 @@
         <v>8945535</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4062,7 +4071,7 @@
         <v>224746957</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4070,7 +4079,7 @@
         <v>16919582</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -4078,7 +4087,7 @@
         <v>2920367</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -4086,7 +4095,7 @@
         <v>39405392</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -4094,7 +4103,7 @@
         <v>194208098</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -4102,7 +4111,7 @@
         <v>294733634</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -4110,7 +4119,7 @@
         <v>59183963</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -4118,7 +4127,7 @@
         <v>17218957</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -4126,7 +4135,7 @@
         <v>125435</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -4134,7 +4143,7 @@
         <v>200253</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -4142,7 +4151,7 @@
         <v>19574608</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -4150,7 +4159,7 @@
         <v>128377539</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -4158,7 +4167,7 @@
         <v>156297</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -4166,7 +4175,7 @@
         <v>3115343</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -4174,7 +4183,7 @@
         <v>4966829</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -4182,7 +4191,7 @@
         <v>16341448</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -4190,7 +4199,7 @@
         <v>2388785</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -4198,7 +4207,7 @@
         <v>39297319</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -4222,13 +4231,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4236,7 +4245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -4244,7 +4253,7 @@
         <v>17560250</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -4252,7 +4261,7 @@
         <v>88942419</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4260,7 +4269,7 @@
         <v>80352022</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -4268,7 +4277,7 @@
         <v>90239860</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -4276,7 +4285,7 @@
         <v>5903464</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -4284,7 +4293,7 @@
         <v>36692192</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -4292,7 +4301,7 @@
         <v>209635043</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4300,7 +4309,7 @@
         <v>59801138</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -4308,7 +4317,7 @@
         <v>1070715</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -4332,13 +4341,13 @@
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4346,439 +4355,439 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B2">
         <v>24515558860</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B3">
         <v>23693590750</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B4">
         <v>21658856186</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B5">
         <v>9532425919</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B6">
         <v>2713167732</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B7">
         <v>423343989</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B8">
         <v>131873086</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B9">
         <v>7905885</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B10">
         <v>2541526880</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B11">
         <v>1202695895</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B12">
         <v>23489362</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B13">
         <v>1659678</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B14">
         <v>1125671998</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B15">
         <v>871417727</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B16">
         <v>780286613</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B17">
         <v>658657789</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B18">
         <v>574769381</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B19">
         <v>551648007</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B20">
         <v>472781797</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B21">
         <v>533612151</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B22">
         <v>352930725</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B23">
         <v>290609292</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B24">
         <v>13263297</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B25">
         <v>2394269</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B26">
         <v>268351495</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B27">
         <v>216449427</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B28">
         <v>202748973</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B29">
         <v>163329883</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B30">
         <v>117495371</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B31">
         <v>98382166</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B32">
         <v>80649563</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B33">
         <v>10082702</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B34">
         <v>1678369</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B35">
         <v>71839953</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B36">
         <v>11363091</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B37">
         <v>5367947</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B38">
         <v>22524</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B39">
         <v>117724592</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B40">
         <v>82327291</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B41">
         <v>1213097</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B42">
         <v>52338869</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B43">
         <v>11219</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B45">
         <v>41926883</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B46">
         <v>17043143</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B47">
         <v>1706998</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B48">
         <v>802625</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B49">
         <v>17940022</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B50">
         <v>4556735</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B51">
         <v>2017930</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B52">
         <v>996128</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B53">
         <v>602672</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B54">
         <v>9267</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B55">
         <v>3489</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>22</v>
       </c>
@@ -4786,9 +4795,9 @@
         <v>18751201</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B57">
         <v>1440818581</v>
@@ -4804,27 +4813,27 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776FD02C-0B59-4710-B819-411B5C9E6AD4}">
-  <dimension ref="A1:G77"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W42" sqref="W42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -4835,7 +4844,7 @@
         <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>28</v>
@@ -4847,7 +4856,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -4870,8 +4879,12 @@
         <f t="shared" ref="G2:G33" si="0">SUM(B2:F2)</f>
         <v>28223508174</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="str">
+        <f>PROPER(A2)</f>
+        <v>Sky</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -4882,8 +4895,12 @@
         <f t="shared" si="0"/>
         <v>24515558860</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H9" si="1">PROPER(A3)</f>
+        <v>Nature Object</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -4894,8 +4911,12 @@
         <f t="shared" si="0"/>
         <v>21658856186</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="str">
+        <f t="shared" si="1"/>
+        <v>Rd Normal Street</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -4912,8 +4933,12 @@
         <f t="shared" si="0"/>
         <v>9575161424</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="str">
+        <f t="shared" si="1"/>
+        <v>Building</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -4933,10 +4958,14 @@
         <f t="shared" si="0"/>
         <v>5536832975</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="str">
+        <f t="shared" si="1"/>
+        <v>Grass</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="F7">
         <v>3276290692</v>
@@ -4945,8 +4974,12 @@
         <f t="shared" si="0"/>
         <v>3276290692</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>Car</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -4960,8 +4993,12 @@
         <f t="shared" si="0"/>
         <v>3100198456</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>Tree</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -4975,10 +5012,14 @@
         <f t="shared" si="0"/>
         <v>2589098189</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>Bush</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="F10">
         <v>2541526880</v>
@@ -4987,10 +5028,14 @@
         <f t="shared" si="0"/>
         <v>2541526880</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="str">
+        <f>PROPER(A10)</f>
+        <v>Sidewalk</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="F11">
         <v>1440818581</v>
@@ -4999,10 +5044,14 @@
         <f t="shared" si="0"/>
         <v>1440818581</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="str">
+        <f t="shared" ref="H11:H74" si="2">PROPER(A11)</f>
+        <v>Ego Car</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F12">
         <v>1227844935</v>
@@ -5011,8 +5060,12 @@
         <f t="shared" si="0"/>
         <v>1227844935</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>Truck</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -5023,8 +5076,12 @@
         <f t="shared" si="0"/>
         <v>1125671998</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>Grid Structure</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -5035,8 +5092,12 @@
         <f t="shared" si="0"/>
         <v>871417727</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v>Road Blocks</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -5047,10 +5108,14 @@
         <f t="shared" si="0"/>
         <v>780286613</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v>Drivable Cobblestone</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="F16">
         <v>658657789</v>
@@ -5059,10 +5124,14 @@
         <f t="shared" si="0"/>
         <v>658657789</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>Curbstone</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F17">
         <v>574769381</v>
@@ -5071,10 +5140,14 @@
         <f t="shared" si="0"/>
         <v>574769381</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v>Solid Line</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F18">
         <v>551648007</v>
@@ -5083,10 +5156,14 @@
         <f t="shared" si="0"/>
         <v>551648007</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>Non Drivable Street</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F19">
         <v>533612151</v>
@@ -5095,10 +5172,14 @@
         <f t="shared" si="0"/>
         <v>533612151</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>Dashed Line</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="F20">
         <v>472781797</v>
@@ -5107,10 +5188,14 @@
         <f t="shared" si="0"/>
         <v>472781797</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>Poles</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F21">
         <v>352930725</v>
@@ -5119,8 +5204,12 @@
         <f t="shared" si="0"/>
         <v>352930725</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>Irrelevant Signs</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -5131,10 +5220,14 @@
         <f t="shared" si="0"/>
         <v>350542071</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v>Mud</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="F23">
         <v>306266858</v>
@@ -5143,10 +5236,14 @@
         <f t="shared" si="0"/>
         <v>306266858</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>Traffic Signs</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E24">
         <v>294733634</v>
@@ -5155,10 +5252,14 @@
         <f t="shared" si="0"/>
         <v>294733634</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>Mulch</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F25">
         <v>268351495</v>
@@ -5167,8 +5268,12 @@
         <f t="shared" si="0"/>
         <v>268351495</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>Parking Area</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -5182,10 +5287,14 @@
         <f t="shared" si="0"/>
         <v>238021596</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>Concrete</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F27">
         <v>216449427</v>
@@ -5194,10 +5303,14 @@
         <f t="shared" si="0"/>
         <v>216449427</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" t="str">
+        <f t="shared" si="2"/>
+        <v>Obstacles Trash</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="C28">
         <v>209635043</v>
@@ -5206,8 +5319,12 @@
         <f t="shared" si="0"/>
         <v>209635043</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>High Vegetation</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>158</v>
       </c>
@@ -5218,10 +5335,14 @@
         <f t="shared" si="0"/>
         <v>202748973</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>Rd Restricted Area</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E30">
         <v>194208098</v>
@@ -5230,8 +5351,12 @@
         <f t="shared" si="0"/>
         <v>194208098</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>Gravel</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>159</v>
       </c>
@@ -5242,8 +5367,12 @@
         <f t="shared" si="0"/>
         <v>163329883</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>Traffic Guide Obj</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -5257,10 +5386,14 @@
         <f t="shared" si="0"/>
         <v>133941019</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" t="str">
+        <f t="shared" si="2"/>
+        <v>Void</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F33">
         <v>117724592</v>
@@ -5269,20 +5402,28 @@
         <f t="shared" si="0"/>
         <v>117724592</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>Painted Driv Instr</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F34">
         <v>117495371</v>
       </c>
       <c r="G34">
-        <f t="shared" ref="G34:G65" si="1">SUM(B34:F34)</f>
+        <f t="shared" ref="G34:G65" si="3">SUM(B34:F34)</f>
         <v>117495371</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" t="str">
+        <f t="shared" si="2"/>
+        <v>Slow Drive Area</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -5293,107 +5434,143 @@
         <v>1070715</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>113051858</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" t="str">
+        <f t="shared" si="2"/>
+        <v>Puddle</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F36">
         <v>98382166</v>
       </c>
       <c r="G36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>98382166</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" t="str">
+        <f t="shared" si="2"/>
+        <v>Signal Corpus</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="F37">
         <v>92410634</v>
       </c>
       <c r="G37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>92410634</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" t="str">
+        <f t="shared" si="2"/>
+        <v>Pedestrian</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>163</v>
       </c>
       <c r="C38">
         <v>90239860</v>
       </c>
       <c r="G38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>90239860</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" t="str">
+        <f t="shared" si="2"/>
+        <v>Rough Trail</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
       <c r="C39">
         <v>88942419</v>
       </c>
       <c r="G39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>88942419</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" t="str">
+        <f t="shared" si="2"/>
+        <v>Smooth Trail</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
       <c r="F40">
         <v>88593515</v>
       </c>
       <c r="G40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>88593515</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" t="str">
+        <f t="shared" si="2"/>
+        <v>Bicycle</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F41">
         <v>83540388</v>
       </c>
       <c r="G41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>83540388</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" t="str">
+        <f t="shared" si="2"/>
+        <v>Utility Vehicle</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D42">
         <v>61190727</v>
       </c>
       <c r="G42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>61190727</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" t="str">
+        <f t="shared" si="2"/>
+        <v>Vegetation</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>166</v>
       </c>
       <c r="E43">
         <v>59183963</v>
       </c>
       <c r="G43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>59183963</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" t="str">
+        <f t="shared" si="2"/>
+        <v>Rock Bed</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -5401,23 +5578,31 @@
         <v>53338450</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>53338450</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" t="str">
+        <f t="shared" si="2"/>
+        <v>Barrier</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F45">
         <v>52350088</v>
       </c>
       <c r="G45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52350088</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45" t="str">
+        <f t="shared" si="2"/>
+        <v>Traffic Signal</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -5428,35 +5613,47 @@
         <v>39405392</v>
       </c>
       <c r="G46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>47730386</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46" t="str">
+        <f t="shared" si="2"/>
+        <v>Asphalt</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="F47">
         <v>41926883</v>
       </c>
       <c r="G47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>41926883</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H47" t="str">
+        <f t="shared" si="2"/>
+        <v>Sidebars</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
       <c r="C48">
         <v>36692192</v>
       </c>
       <c r="G48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>36692192</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48" t="str">
+        <f t="shared" si="2"/>
+        <v>Low Vegetation</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -5464,11 +5661,15 @@
         <v>26891615</v>
       </c>
       <c r="G49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>26891615</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H49" t="str">
+        <f t="shared" si="2"/>
+        <v>Rubble</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -5479,11 +5680,15 @@
         <v>19574608</v>
       </c>
       <c r="G50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>24020217</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50" t="str">
+        <f t="shared" si="2"/>
+        <v>Fence</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -5494,11 +5699,15 @@
         <v>16919582</v>
       </c>
       <c r="G51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>21808904</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51" t="str">
+        <f t="shared" si="2"/>
+        <v>Vehicle</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -5509,13 +5718,17 @@
         <v>8945535</v>
       </c>
       <c r="G52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>20756688</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52" t="str">
+        <f t="shared" si="2"/>
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="B53">
         <v>118476</v>
@@ -5533,35 +5746,47 @@
         <v>18751201</v>
       </c>
       <c r="G53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>20175699</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53" t="str">
+        <f t="shared" si="2"/>
+        <v>Unknown Error</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F54">
         <v>17940022</v>
       </c>
       <c r="G54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>17940022</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H54" t="str">
+        <f t="shared" si="2"/>
+        <v>Zebra Crossing</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C55">
         <v>17560250</v>
       </c>
       <c r="G55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>17560250</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H55" t="str">
+        <f t="shared" si="2"/>
+        <v>Background</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -5569,23 +5794,31 @@
         <v>17218957</v>
       </c>
       <c r="G56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>17218957</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56" t="str">
+        <f t="shared" si="2"/>
+        <v>Log</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D57">
         <v>13732978</v>
       </c>
       <c r="G57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>13732978</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57" t="str">
+        <f t="shared" si="2"/>
+        <v>Trail</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -5596,35 +5829,47 @@
         <v>200253</v>
       </c>
       <c r="G58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8992249</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H58" t="str">
+        <f t="shared" si="2"/>
+        <v>Person</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F59">
         <v>6517588.6670000004</v>
       </c>
       <c r="G59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6517588.6670000004</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H59" t="str">
+        <f t="shared" si="2"/>
+        <v>Small Vehicles</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C60">
         <v>5903464</v>
       </c>
       <c r="G60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5903464</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H60" t="str">
+        <f t="shared" si="2"/>
+        <v>Obstacle</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -5635,23 +5880,31 @@
         <v>5133510</v>
       </c>
       <c r="G61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5143569</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H61" t="str">
+        <f t="shared" si="2"/>
+        <v>Dirt</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E62">
         <v>4966829</v>
       </c>
       <c r="G62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4966829</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H62" t="str">
+        <f t="shared" si="2"/>
+        <v>Bridge</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -5662,11 +5915,15 @@
         <v>441762</v>
       </c>
       <c r="G63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4854313</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H63" t="str">
+        <f t="shared" si="2"/>
+        <v>Object</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>51</v>
       </c>
@@ -5677,11 +5934,15 @@
         <v>2299774</v>
       </c>
       <c r="G64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4801689</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H64" t="str">
+        <f t="shared" si="2"/>
+        <v>Pole</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>58</v>
       </c>
@@ -5689,152 +5950,204 @@
         <v>4718316</v>
       </c>
       <c r="G65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4718316</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H65" t="str">
+        <f t="shared" si="2"/>
+        <v>Log</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="F66">
         <v>4556735</v>
       </c>
       <c r="G66">
-        <f t="shared" ref="G66:G97" si="2">SUM(B66:F66)</f>
+        <f t="shared" ref="G66:G77" si="4">SUM(B66:F66)</f>
         <v>4556735</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H66" t="str">
+        <f t="shared" si="2"/>
+        <v>Electronic Traffic</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E67">
         <v>4512457</v>
       </c>
       <c r="G67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4512457</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H67" t="str">
+        <f t="shared" si="2"/>
+        <v>Sand</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E68">
         <v>3115343</v>
       </c>
       <c r="G68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3115343</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H68" t="str">
+        <f t="shared" si="2"/>
+        <v>Rock</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>173</v>
       </c>
       <c r="E69">
         <v>2920367</v>
       </c>
       <c r="G69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2920367</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H69" t="str">
+        <f t="shared" si="2"/>
+        <v>Container &amp; Generic Object</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>174</v>
       </c>
       <c r="E70">
         <v>2388785</v>
       </c>
       <c r="G70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2388785</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H70" t="str">
+        <f t="shared" si="2"/>
+        <v>Picnic Table</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="F71">
         <v>2017930</v>
       </c>
       <c r="G71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2017930</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H71" t="str">
+        <f t="shared" si="2"/>
+        <v>Tractor</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="F72">
         <v>996128</v>
       </c>
       <c r="G72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>996128</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H72" t="str">
+        <f t="shared" si="2"/>
+        <v>Blurred Area</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="F73">
         <v>602672</v>
       </c>
       <c r="G73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>602672</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H73" t="str">
+        <f t="shared" si="2"/>
+        <v>Animals</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E74">
         <v>156297</v>
       </c>
       <c r="G74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>156297</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H74" t="str">
+        <f t="shared" si="2"/>
+        <v>Sign</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E75">
         <v>125435</v>
       </c>
       <c r="G75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>125435</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H75" t="str">
+        <f t="shared" ref="H75:H77" si="5">PROPER(A75)</f>
+        <v>Bicyle</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="F76">
         <v>9267</v>
       </c>
       <c r="G76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9267</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H76" t="str">
+        <f t="shared" si="5"/>
+        <v>Speed Bumper</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="F77">
         <v>3489</v>
       </c>
       <c r="G77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3489</v>
+      </c>
+      <c r="H77" t="str">
+        <f t="shared" si="5"/>
+        <v>Rain Dirt</v>
       </c>
     </row>
   </sheetData>

</xml_diff>